<commit_message>
Fix input wrong semester upload activity
</commit_message>
<xml_diff>
--- a/public/files/Activities.xlsx
+++ b/public/files/Activities.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\MyWork\satit\Extra\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Excel sheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Excel sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+  <si>
+    <t>Academic Year</t>
+  </si>
+  <si>
+    <t>Grade Level</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
   <si>
     <t>Fill these cells in with S, U, or leave blank</t>
   </si>
@@ -23,40 +36,37 @@
     <t>Activities</t>
   </si>
   <si>
-    <t>Homeroom 5</t>
-  </si>
-  <si>
-    <t>Extra Curricular Activities 5</t>
-  </si>
-  <si>
-    <t>Guidance and Developmental Skills 5</t>
-  </si>
-  <si>
-    <t>Social Spirit 5</t>
-  </si>
-  <si>
-    <t>Shadowing</t>
-  </si>
-  <si>
-    <t>Newspaper</t>
-  </si>
-  <si>
-    <t>Yearbook</t>
-  </si>
-  <si>
-    <t>Homeroom 6</t>
-  </si>
-  <si>
-    <t>Extra Curricular Activities 6</t>
-  </si>
-  <si>
-    <t>Guidance and Developmental Skills 6</t>
-  </si>
-  <si>
-    <t>Social Spirit 6</t>
-  </si>
-  <si>
-    <t>No.</t>
+    <t>Day Camp 1</t>
+  </si>
+  <si>
+    <t>Social Spirit 1</t>
+  </si>
+  <si>
+    <t>Homeroom 1</t>
+  </si>
+  <si>
+    <t>Extra Curricular Activities 1</t>
+  </si>
+  <si>
+    <t>Cultural Activities 1</t>
+  </si>
+  <si>
+    <t>Course ID</t>
+  </si>
+  <si>
+    <t>DCAMP 1</t>
+  </si>
+  <si>
+    <t>SS 11</t>
+  </si>
+  <si>
+    <t>ก 11913</t>
+  </si>
+  <si>
+    <t>ก 11923</t>
+  </si>
+  <si>
+    <t>ก 11933</t>
   </si>
   <si>
     <t>Students ID</t>
@@ -68,23 +78,131 @@
     <t>1st Semester</t>
   </si>
   <si>
-    <t>2nd Semester</t>
+    <t>2st Semester</t>
+  </si>
+  <si>
+    <t>Apisada Sangkhasap</t>
+  </si>
+  <si>
+    <t>Arissara Wuthisasna</t>
+  </si>
+  <si>
+    <t>Asawin Srisuphapreeda</t>
+  </si>
+  <si>
+    <t>Chakree Kenganantanon</t>
+  </si>
+  <si>
+    <t>Grace Tirachulisoonthorn</t>
+  </si>
+  <si>
+    <t>Jiratthaya Jirarojwong</t>
+  </si>
+  <si>
+    <t>KevinWongsamut Tiyatha</t>
+  </si>
+  <si>
+    <t>Lawitra Sitapan</t>
+  </si>
+  <si>
+    <t>Leartrat Tangvongleart</t>
+  </si>
+  <si>
+    <t>Manutchanika Paitoonrajitpipit</t>
+  </si>
+  <si>
+    <t>Naphat Thanaphan</t>
+  </si>
+  <si>
+    <t>Narawadee Jermnarong</t>
+  </si>
+  <si>
+    <t>Natrada Jermnarong</t>
+  </si>
+  <si>
+    <t>Natthanicha Boonchu</t>
+  </si>
+  <si>
+    <t>OrnthibhaHomsettee Lertbannaphong</t>
+  </si>
+  <si>
+    <t>Pathomtat Niponpittaya</t>
+  </si>
+  <si>
+    <t>Phraephan Chantana</t>
+  </si>
+  <si>
+    <t>Pun Pichedpan</t>
+  </si>
+  <si>
+    <t>Putthipat Trivisvavet</t>
+  </si>
+  <si>
+    <t>Satakoon Sasirathsiri</t>
+  </si>
+  <si>
+    <t>Setthawut Sitthipitaks</t>
+  </si>
+  <si>
+    <t>Shina Sastrawaha</t>
+  </si>
+  <si>
+    <t>Swishakorn Singkul</t>
+  </si>
+  <si>
+    <t>Thanakorn Theppattra</t>
+  </si>
+  <si>
+    <t>Thanakrit Pengsri</t>
+  </si>
+  <si>
+    <t>Tharadol Phoothong</t>
+  </si>
+  <si>
+    <t>Thianwit Jerapornprapa</t>
+  </si>
+  <si>
+    <t>Emily Tomlinson</t>
+  </si>
+  <si>
+    <t>Warisara Jintanawan</t>
+  </si>
+  <si>
+    <t>Watchanon Wattanabunyongcharoen</t>
+  </si>
+  <si>
+    <t>Promphan Songwatcharaporn</t>
+  </si>
+  <si>
+    <t>Melisa Tunchumrus</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Tw Cen MT"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -92,10 +210,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -111,7 +226,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -125,42 +246,47 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,149 +576,507 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AN3"/>
+  <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="true" style="0"/>
-    <col min="3" max="3" width="19" customWidth="true" style="0"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:40">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="6" t="s">
+      <c r="B1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:40" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+    </row>
+    <row r="6" spans="1:40" ht="27" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-    </row>
-    <row r="3" spans="1:40">
-      <c r="A3" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="H6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2600081170</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2600081171</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2600081172</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2600081173</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2600081174</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2600081175</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2600081176</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2600081177</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2600081178</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2600081179</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2600081180</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2600081181</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2600081182</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2600081184</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2600081185</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2600081186</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2600081187</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2600081188</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2600081189</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2600081190</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2600081191</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2600081192</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2600081193</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2600081194</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2600081195</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2600081196</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2600081197</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2600081200</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2600081201</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2600081202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2610181247</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2610181248</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="A1:D1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="3">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="A4:D4"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>